<commit_message>
Temp code to query google maps
Query google maps and save to excel spreadsheet for use throughout project instead of continuing to query google since we only have 3000/day.
</commit_message>
<xml_diff>
--- a/CBD/bin/Debug/Locations.xlsx
+++ b/CBD/bin/Debug/Locations.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klevi18\Desktop\CBDBuses-master\CBD\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kath\Desktop\CBDBuses-master\CBD\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14150"/>
   </bookViews>
   <sheets>
     <sheet name="Placements" sheetId="1" r:id="rId1"/>
     <sheet name="Buses" sheetId="2" r:id="rId2"/>
     <sheet name="Distances" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="268">
   <si>
     <t>Organization</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Location 1</t>
   </si>
   <si>
-    <t xml:space="preserve">320 E. Second Ave. </t>
-  </si>
-  <si>
     <t>Elizabeth</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Arc of Spokane Valley</t>
   </si>
   <si>
-    <t>10814 E. Broadway Ave.</t>
-  </si>
-  <si>
     <t>Cris</t>
   </si>
   <si>
@@ -104,9 +98,6 @@
   </si>
   <si>
     <t>Christ Kitchen</t>
-  </si>
-  <si>
-    <t>2410 N. Monroe Street</t>
   </si>
   <si>
     <t>Mike</t>
@@ -143,9 +134,6 @@
   </si>
   <si>
     <t>Food For All</t>
-  </si>
-  <si>
-    <t>1635 W 26th Ave</t>
   </si>
   <si>
     <t>Aaron</t>
@@ -190,9 +178,6 @@
     <t>Goodwill North</t>
   </si>
   <si>
-    <t>9832 N Nevada</t>
-  </si>
-  <si>
     <t>Celisse</t>
   </si>
   <si>
@@ -200,9 +185,6 @@
   </si>
   <si>
     <t>Goodwill South</t>
-  </si>
-  <si>
-    <t>130 E 3rd Avenue</t>
   </si>
   <si>
     <t>Sardinia</t>
@@ -274,9 +256,6 @@
     <t>Lilac Services for the Blind</t>
   </si>
   <si>
-    <t>1212 N Howard St</t>
-  </si>
-  <si>
     <t>Kent</t>
   </si>
   <si>
@@ -284,9 +263,6 @@
   </si>
   <si>
     <t>MAC</t>
-  </si>
-  <si>
-    <t>2316 West First Avenue\Spokane, WA 99201</t>
   </si>
   <si>
     <t>Katie</t>
@@ -298,9 +274,6 @@
     <t>Mission Community Outreach</t>
   </si>
   <si>
-    <t>1906 E Mission Ave\Spokane, WA 99202</t>
-  </si>
-  <si>
     <t>Lindy</t>
   </si>
   <si>
@@ -308,9 +281,6 @@
   </si>
   <si>
     <t>New Hope Resource Center</t>
-  </si>
-  <si>
-    <t>4211 E. Colbert Rd\Colbert WA  99005</t>
   </si>
   <si>
     <t>Stacy</t>
@@ -322,9 +292,6 @@
     <t>Northeast Youth Center</t>
   </si>
   <si>
-    <t>3004 E. Queen Ave</t>
-  </si>
-  <si>
     <t>Laura</t>
   </si>
   <si>
@@ -332,9 +299,6 @@
   </si>
   <si>
     <t>Our Place Ministries</t>
-  </si>
-  <si>
-    <t>1509 W College \Spokane, WA 99201</t>
   </si>
   <si>
     <t>Karen</t>
@@ -376,9 +340,6 @@
     <t>SCRAPS</t>
   </si>
   <si>
-    <t>6815 E. Trent Avenue\Spokane Valley, WA 99212</t>
-  </si>
-  <si>
     <t>Joy</t>
   </si>
   <si>
@@ -388,9 +349,6 @@
     <t>Second Harvest</t>
   </si>
   <si>
-    <t>1234 E Front Ave\Spokane, WA\99202</t>
-  </si>
-  <si>
     <t>Dale</t>
   </si>
   <si>
@@ -398,9 +356,6 @@
   </si>
   <si>
     <t>Shadle Park</t>
-  </si>
-  <si>
-    <t>5508 N. Alberta St.\Spokane, WA 99205\(and possibly at homes nearby)</t>
   </si>
   <si>
     <t>Wyma</t>
@@ -511,9 +466,6 @@
     <t>Group4</t>
   </si>
   <si>
-    <t>9907 E. Wellesley Avenue</t>
-  </si>
-  <si>
     <t>Size4</t>
   </si>
   <si>
@@ -532,9 +484,6 @@
     <t>Spots remaining</t>
   </si>
   <si>
-    <t>1120 W. Sprague Ave. Cathedral Plaza</t>
-  </si>
-  <si>
     <t>Matt</t>
   </si>
   <si>
@@ -544,9 +493,6 @@
     <t>Volunteer Chore Services: Fahy West</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1523 W. Dean/1411 W. Dean Fahy West Gardens</t>
-  </si>
-  <si>
     <t>Rafeal</t>
   </si>
   <si>
@@ -554,9 +500,6 @@
   </si>
   <si>
     <t>Volunteer Chore Services: O'Malley Apts</t>
-  </si>
-  <si>
-    <t>707 E. Mission Ave O"Malley Apts</t>
   </si>
   <si>
     <t>Kirk</t>
@@ -569,9 +512,6 @@
   </si>
   <si>
     <t>4211 E. Colbert Rd, Colbert,  WA 99005</t>
-  </si>
-  <si>
-    <t>4603 N. Market\Spokane WA, 99207</t>
   </si>
   <si>
     <t>Cynthia</t>
@@ -822,12 +762,99 @@
   <si>
     <t>318 S. Cedar St Spokane, WA</t>
   </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Whitworth University</t>
+  </si>
+  <si>
+    <t>300 W Hawthorne Rd Spokane, WA 99251</t>
+  </si>
+  <si>
+    <t>320 E. Second Ave. Spokane, WA</t>
+  </si>
+  <si>
+    <t>4603 N. Market Spokane WA, 99207</t>
+  </si>
+  <si>
+    <t>707 E. Mission Ave Spokane, WA</t>
+  </si>
+  <si>
+    <t>1120 W. Sprague Ave. Spokane, WA</t>
+  </si>
+  <si>
+    <t>9907 E. Wellesley Avenue Spokane, WA</t>
+  </si>
+  <si>
+    <t>101 E. Hartson Spokane, WA</t>
+  </si>
+  <si>
+    <t>W. 19 Pacific Spokane, WA</t>
+  </si>
+  <si>
+    <t>25 W. 5th Avenue Spokane, WA</t>
+  </si>
+  <si>
+    <t>6607 N. Havana Spokane, WA</t>
+  </si>
+  <si>
+    <t>1212 N Howard St Spokane, WA</t>
+  </si>
+  <si>
+    <t>130 E 3rd Avenue Spokane, WA</t>
+  </si>
+  <si>
+    <t>9832 N Nevada Spokane, WA</t>
+  </si>
+  <si>
+    <t>1635 W 26th Ave Spokane, WA</t>
+  </si>
+  <si>
+    <t>2410 N. Monroe Street Spokane, WA</t>
+  </si>
+  <si>
+    <t>10814 E. Broadway Ave. Spokane, WA</t>
+  </si>
+  <si>
+    <t>32 West Pacific Ave. Spokane, WA</t>
+  </si>
+  <si>
+    <t>2316 West First Avenue Spokane, WA 99201</t>
+  </si>
+  <si>
+    <t>1906 E Mission Ave Spokane, WA 99202</t>
+  </si>
+  <si>
+    <t>1509 W College Spokane, WA 99201</t>
+  </si>
+  <si>
+    <t>6815 E. Trent Avenue Spokane Valley, WA 99212</t>
+  </si>
+  <si>
+    <t>1234 E Front Ave Spokane, WA 99202</t>
+  </si>
+  <si>
+    <t>5508 N. Alberta St. Spokane, WA 99205</t>
+  </si>
+  <si>
+    <t>1411 W. Dean  Spokane, WA</t>
+  </si>
+  <si>
+    <t>4211 E. Colbert Rd Colbert, WA  99005</t>
+  </si>
+  <si>
+    <t>3004 E. Queen Ave Spokane, WA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -860,6 +887,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -925,7 +959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -953,6 +987,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -967,8 +1002,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -997,7 +1060,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvPr id="1026" name="Rectangle 2" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1040,7 +1109,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1088,7 +1163,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 2"/>
+        <xdr:cNvPr id="3" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1136,7 +1217,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvPr id="4" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1248,6 +1335,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1283,6 +1387,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1437,19 +1558,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="26" width="7.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.453125" customWidth="1"/>
+    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="3" max="3" width="15.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
+    <col min="7" max="26" width="7.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1477,13 +1598,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6">
         <v>19</v>
@@ -1494,16 +1615,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="9">
         <v>14</v>
@@ -1514,16 +1635,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="E4" s="6">
         <v>18</v>
@@ -1534,16 +1655,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E5" s="6">
         <v>8</v>
@@ -1554,16 +1675,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E6" s="9">
         <v>20</v>
@@ -1574,16 +1695,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>255</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E7" s="6">
         <v>19</v>
@@ -1594,16 +1715,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E8" s="9">
         <v>18</v>
@@ -1614,16 +1735,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="D9" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="E9" s="6">
         <v>26</v>
@@ -1634,16 +1755,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E10" s="9">
         <v>18</v>
@@ -1654,16 +1775,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>48</v>
+        <v>254</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E11" s="6">
         <v>16</v>
@@ -1674,16 +1795,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>52</v>
+        <v>253</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E12" s="9">
         <v>23</v>
@@ -1694,16 +1815,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E13" s="6">
         <v>20</v>
@@ -1714,16 +1835,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E14" s="9">
         <v>18</v>
@@ -1734,16 +1855,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="E15" s="6">
         <v>25</v>
@@ -1754,16 +1875,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>61</v>
-      </c>
       <c r="D16" s="9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E16" s="9">
         <v>18</v>
@@ -1774,16 +1895,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>64</v>
+        <v>258</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E17" s="6">
         <v>14</v>
@@ -1794,16 +1915,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="E18" s="9">
         <v>20</v>
@@ -1814,16 +1935,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E19" s="6">
         <v>19</v>
@@ -1834,16 +1955,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>76</v>
+        <v>252</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E20" s="9">
         <v>18</v>
@@ -1854,16 +1975,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>80</v>
+        <v>259</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E21" s="6">
         <v>19</v>
@@ -1874,16 +1995,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="11" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>84</v>
+        <v>260</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E22" s="9">
         <v>18</v>
@@ -1894,16 +2015,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>88</v>
+        <v>266</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="E23" s="6">
         <v>18</v>
@@ -1914,16 +2035,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>92</v>
+        <v>267</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E24" s="9">
         <v>14</v>
@@ -1934,16 +2055,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>96</v>
+        <v>261</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E25" s="6">
         <v>20</v>
@@ -1954,16 +2075,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="E26" s="9">
         <v>12</v>
@@ -1974,16 +2095,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="5" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E27" s="6">
         <v>22</v>
@@ -1994,16 +2115,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>110</v>
+        <v>262</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="E28" s="9">
         <v>18</v>
@@ -2014,16 +2135,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="5" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>114</v>
+        <v>263</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E29" s="6">
         <v>18</v>
@@ -2034,16 +2155,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="7" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>118</v>
+        <v>264</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="E30" s="9">
         <v>20</v>
@@ -2054,16 +2175,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="5" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="E31" s="6">
         <v>19</v>
@@ -2074,16 +2195,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="7" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>125</v>
+        <v>251</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E32" s="9">
         <v>19</v>
@@ -2094,16 +2215,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="5" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="6">
@@ -2112,16 +2233,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="7" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>134</v>
+        <v>250</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="E34" s="9">
         <v>13</v>
@@ -2132,16 +2253,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="5" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>142</v>
+        <v>249</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E35" s="6">
         <v>12</v>
@@ -2152,16 +2273,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="7" t="s">
-        <v>257</v>
+        <v>237</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>148</v>
+        <v>248</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E36" s="9">
         <v>18</v>
@@ -2172,16 +2293,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>155</v>
+        <v>247</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="E37" s="6">
         <v>9</v>
@@ -2192,16 +2313,16 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="11" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>162</v>
+        <v>246</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="E38" s="9">
         <v>22</v>
@@ -2212,16 +2333,16 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="5" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>166</v>
+        <v>265</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="E39" s="6">
         <v>19</v>
@@ -2232,16 +2353,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="11" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>170</v>
+        <v>245</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="E40" s="9">
         <v>14</v>
@@ -2252,16 +2373,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>175</v>
+        <v>244</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="E41" s="6">
         <v>18</v>
@@ -2271,8 +2392,12 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
+      <c r="A42" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>242</v>
+      </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -9947,51 +10072,51 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
-    <col min="15" max="18" width="12.140625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="8.28515625" customWidth="1"/>
-    <col min="21" max="22" width="11.42578125" customWidth="1"/>
-    <col min="23" max="27" width="7.7109375" customWidth="1"/>
-    <col min="28" max="28" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="10" max="10" width="12.1796875" customWidth="1"/>
+    <col min="11" max="11" width="16.1796875" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="12.1796875" customWidth="1"/>
+    <col min="15" max="18" width="12.1796875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1796875" customWidth="1"/>
+    <col min="20" max="20" width="8.26953125" customWidth="1"/>
+    <col min="21" max="22" width="11.453125" customWidth="1"/>
+    <col min="23" max="27" width="7.7265625" customWidth="1"/>
+    <col min="28" max="28" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="19" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="22"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
@@ -9999,22 +10124,22 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="V1" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W1" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="X1" s="10"/>
-      <c r="Y1" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
+      <c r="Y1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
       <c r="AB1" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:28">
@@ -10022,61 +10147,61 @@
         <v>5</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="G2" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="J2" s="15" t="s">
+      <c r="N2" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q2" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="L2" s="13" t="s">
+      <c r="R2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="P2" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="10"/>
@@ -10092,37 +10217,37 @@
         <v>58</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="F3" s="5">
         <v>18</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="J3" s="5">
         <v>20</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="N3" s="4">
         <v>19</v>
@@ -10146,7 +10271,7 @@
         <v>1</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="X3" s="10"/>
       <c r="AB3" s="2"/>
@@ -10162,34 +10287,34 @@
         <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="F4" s="7">
         <v>19</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="J4" s="7">
         <v>19</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="N4" s="7">
         <v>18</v>
@@ -10211,7 +10336,7 @@
       </c>
       <c r="V4" s="10"/>
       <c r="W4" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="X4" s="10"/>
       <c r="AB4" s="2"/>
@@ -10224,26 +10349,26 @@
         <v>56</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="F5" s="5">
         <f>18+18</f>
         <v>36</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="J5" s="5">
         <v>18</v>
@@ -10271,7 +10396,7 @@
         <v>2</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="X5" s="10"/>
       <c r="AB5" s="2"/>
@@ -10284,37 +10409,37 @@
         <v>55</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="F6" s="7">
         <v>18</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="J6" s="7">
         <v>14</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="N6" s="7">
         <v>18</v>
@@ -10336,7 +10461,7 @@
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="X6" s="10"/>
       <c r="AB6" s="2"/>
@@ -10349,25 +10474,25 @@
         <v>55</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="F7" s="5">
         <v>22</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="J7" s="5">
         <v>19</v>
@@ -10393,7 +10518,7 @@
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="X7" s="10"/>
       <c r="AB7" s="2"/>
@@ -10406,25 +10531,25 @@
         <v>55</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="F8" s="7">
         <v>14</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="J8" s="7">
         <v>23</v>
@@ -10452,7 +10577,7 @@
         <v>1</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="X8" s="10"/>
       <c r="AB8" s="2"/>
@@ -10465,25 +10590,25 @@
         <v>55</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="F9" s="5">
         <v>16</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="J9" s="5">
         <v>20</v>
@@ -10509,7 +10634,7 @@
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="X9" s="10"/>
       <c r="AB9" s="2"/>
@@ -10522,25 +10647,25 @@
         <v>55</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="F10" s="11">
         <v>14</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="J10" s="11">
         <v>18</v>
@@ -10566,7 +10691,7 @@
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
@@ -10582,37 +10707,37 @@
         <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="F11" s="5">
         <v>20</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="J11" s="5">
         <v>12</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="N11" s="5">
         <v>8</v>
@@ -10636,7 +10761,7 @@
         <v>2</v>
       </c>
       <c r="W11" s="10" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="X11" s="10"/>
       <c r="AB11" s="2"/>
@@ -10649,25 +10774,25 @@
         <v>55</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="F12" s="11">
         <v>19</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="J12" s="11">
         <v>19</v>
@@ -10695,7 +10820,7 @@
         <v>1</v>
       </c>
       <c r="W12" s="10" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="X12" s="10"/>
       <c r="AB12" s="2"/>
@@ -10708,25 +10833,25 @@
         <v>55</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
       <c r="F13" s="4">
         <v>26</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="J13" s="4">
         <v>18</v>
@@ -10752,7 +10877,7 @@
       </c>
       <c r="V13" s="10"/>
       <c r="W13" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="X13" s="10"/>
       <c r="Y13" s="10"/>
@@ -10768,37 +10893,37 @@
         <v>48</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>235</v>
+        <v>215</v>
       </c>
       <c r="F14" s="11">
         <v>9</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="J14" s="11">
         <v>18</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="N14" s="11">
         <v>14</v>
@@ -10820,7 +10945,7 @@
       </c>
       <c r="V14" s="10"/>
       <c r="W14" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="X14" s="10"/>
       <c r="AB14" s="2"/>
@@ -10833,23 +10958,23 @@
         <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="F15" s="5">
         <v>18</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="J15" s="5">
         <v>25</v>
@@ -10877,7 +11002,7 @@
         <v>4</v>
       </c>
       <c r="W15" s="10" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="X15" s="10"/>
       <c r="AB15" s="2"/>
@@ -10890,23 +11015,23 @@
         <v>48</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="F16" s="7">
         <v>18</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="J16" s="7">
         <v>20</v>
@@ -10934,7 +11059,7 @@
         <v>9</v>
       </c>
       <c r="W16" s="10" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="X16" s="10"/>
       <c r="AB16" s="2"/>
@@ -10947,37 +11072,37 @@
         <v>47</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>246</v>
+        <v>226</v>
       </c>
       <c r="F17" s="5">
         <v>13</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="J17" s="5">
         <v>10</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>248</v>
+        <v>228</v>
       </c>
       <c r="N17" s="5">
         <v>18</v>
@@ -11001,7 +11126,7 @@
         <v>1</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="AB17" s="2"/>
     </row>
@@ -11013,25 +11138,25 @@
         <v>31</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="F18" s="11">
         <v>19</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>252</v>
+        <v>232</v>
       </c>
       <c r="J18" s="7">
         <v>11</v>
@@ -11057,7 +11182,7 @@
       </c>
       <c r="V18" s="10"/>
       <c r="W18" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="AB18" s="2"/>
     </row>
@@ -11069,13 +11194,13 @@
         <v>29</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>253</v>
+        <v>233</v>
       </c>
       <c r="F19" s="5">
         <v>22</v>
@@ -11105,7 +11230,7 @@
       </c>
       <c r="V19" s="10"/>
       <c r="W19" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="AB19" s="2"/>
     </row>
@@ -11117,13 +11242,13 @@
         <v>27</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>254</v>
+        <v>234</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>255</v>
+        <v>235</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>256</v>
+        <v>236</v>
       </c>
       <c r="F20" s="11">
         <v>20</v>
@@ -11153,7 +11278,7 @@
       </c>
       <c r="V20" s="10"/>
       <c r="W20" s="10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="AB20" s="2"/>
     </row>
@@ -35672,12 +35797,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="30.08984375" customWidth="1"/>
+    <col min="2" max="2" width="47.6328125" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>